<commit_message>
Merged data sets. species & indv mixing models
</commit_message>
<xml_diff>
--- a/data/UW_BothelSI.xlsx
+++ b/data/UW_BothelSI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebekahstiling/Desktop/RProjects/WAlakefoodwebCN/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA7BF86-58C9-5E4B-BC46-95D3C3496188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EE55EF-900E-F14A-9750-3F7BF7BD1E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2420" yWindow="-20280" windowWidth="27640" windowHeight="16440" xr2:uid="{A6B8D408-9616-DF4C-87E4-F719914B2B68}"/>
   </bookViews>
@@ -1081,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9076E9D-CF94-DB4F-98DB-BC5E08AD9FF2}">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2883,7 +2883,7 @@
         <v>106</v>
       </c>
       <c r="B45">
-        <v>1900</v>
+        <v>2019</v>
       </c>
       <c r="C45" t="s">
         <v>37</v>

</xml_diff>